<commit_message>
Update methods and figure 6
</commit_message>
<xml_diff>
--- a/SupplementaryData/SupplementaryData1.xlsx
+++ b/SupplementaryData/SupplementaryData1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfa/Dropbox (MIT)/Paper-ASO-SEISMIC/SupplementaryData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mfa/Dropbox (HMS)/csb/Paper-ASO-SEISMIC/SupplementaryData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA9B5CBA-D704-8647-B497-8EF6387C5ABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42AE6A21-054A-454D-8465-9ED295F117B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="1380" windowWidth="28040" windowHeight="17440" xr2:uid="{2E01D5A3-FB42-A244-9A96-6A1858AC817E}"/>
+    <workbookView xWindow="4160" yWindow="1380" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{2E01D5A3-FB42-A244-9A96-6A1858AC817E}"/>
   </bookViews>
   <sheets>
     <sheet name="Primers" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="226">
   <si>
     <t>Name</t>
   </si>
@@ -48,9 +48,6 @@
     <t>Sequence</t>
   </si>
   <si>
-    <t>SARS2_3kb</t>
-  </si>
-  <si>
     <t>AATAATGAGCTTAGTCCTGTTGCACTACGACAGATGTCTTGTGCTGCCGGTACTACACAAACTGCTTGCACTGATGACAATGCGTTAGCTTACTACAACACAACAAAGGGAGGTAGGTTTGTACTTGCACTGTTATCCGATTTACAGGATTTGAAATGGGCTAGATTCCCTAAGAGTGATGGAACTGGTACTATCTATACAGAACTGGAACCACCTTGTAGGTTTGTTACAGACACACCTAAAGGTCCTAAAGTGAAGTATTTATACTTTATTAAAGGATTAAACAACCTAAATAGAGGTATGGTACTTGGTAGTTTAGCTGCCACAGTACGTCTACAAGCTGGTAATGCAACAGAAGTGCCTGCCAATTCAACTGTATTATCTTTCTGTGCTTTTGCTGTAGATGCTGCTAAAGCTTACAAAGATTATCTAGCTAGTGGGGGACAACCAATCACTAATTGTGTTAAGATGTTGTGTACACACACTGGTACTGGTCAGGCAATAACAGTTACACCGGAAGCCAATATGGATCAAGAATCCTTTGGTGGTGCATCGTGTTGTCTGTACTGCCGTTGCCACATAGATCATCCAAATCCTAAAGGATTTTGTGACTTAAAAGGTAAGTATGTACAAATACCTACAACTTGTGCTAATGACCCTGTGGGTTTTACACTTAAAAACACAGTCTGTACCGTCTGCGGTATGTGGAAAGGTTATGGCTGTAGTTGTGATCAACTCCGCGAACCCATGCTTCAGTCAGCTGATGCACAATCGTTTTTAAACGGGTTTGCGGTGTAAGTGCAGCCCGTCTTACACCGTGCGGCACAGGCACTAGTACTGATGTCGTATACAGGGCTTTTGACATCTACAATGATAAAGTAGCTGGTTTTGCTAAATTCCTAAAAACTAATTGTTGTCGCTTCCAAGAAAAGGACGAAGATGACAATTTAATTGATTCTTACTTTGTAGTTAAGAGACACACTTTCTCTAACTACCAACATGAAGAAACAATTTATAATTTACTTAAGGATTGTCCAGCTGTTGCTAAACATGACTTCTTTAAGTTTAGAATAGACGGTGACATGGTACCACATATATCACGTCAACGTCTTACTAAATACACAATGGCAGACCTCGTCTATGCTTTAAGGCATTTTGATGAAGGTAATTGTGACACATTAAAAGAAATACTTGTCACATACAATTGTTGTGATGATGATTATTTCAATAAAAAGGACTGGTATGATTTTGTAGAAAACCCAGATATATTACGCGTATACGCCAACTTAGGTGAACGTGTACGCCAAGCTTTGTTAAAAACAGTACAATTCTGTGATGCCATGCGAAATGCTGGTATTGTTGGTGTACTGACATTAGATAATCAAGATCTCAATGGTAACTGGTATGATTTCGGTGATTTCATACAAACCACGCCAGGTAGTGGAGTTCCTGTTGTAGATTCTTATTATTCATTGTTAATGCCTATATTAACCTTGACCAGGGCTTTAACTGCAGAGTCACATGTTGACACTGACTTAACAAAGCCTTACATTAAGTGGGATTTGTTAAAATATGACTTCACGGAAGAGAGGTTAAAACTCTTTGACCGTTATTTTAAATATTGGGATCAGACATACCACCCAAATTGTGTTAACTGTTTGGATGACAGATGCATTCTGCATTGTGCAAACTTTAATGTTTTATTCTCTACAGTGTTCCCACCTACAAGTTTTGGACCACTAGTGAGAAAAATATTTGTTGATGGTGTTCCATTTGTAGTTTCAACTGGATACCACTTCAGAGAGCTAGGTGTTGTACATAATCAGGATGTAAACTTACATAGCTCTAGACTTAGTTTTAAGGAATTACTTGTGTATGCTGCTGACCCTGCTATGCACGCTGCTTCTGGTAATCTATTACTAGATAAACGCACTACGTGCTTTTCAGTAGCTGCACTTACTAACAATGTTGCTTTTCAAACTGTCAAACCCGGTAATTTTAACAAAGACTTCTATGACTTTGCTGTGTCTAAGGGTTTCTTTAAGGAAGGAAGTTCTGTTGAATTAAAACACTTCTTCTTTGCTCAGGATGGTAATGCTGCTATCAGCGATTATGACTACTATCGTTATAATCTACCAACAATGTGTGATATCAGACAACTACTATTTGTAGTTGAAGTTGTTGATAAGTACTTTGATTGTTACGATGGTGGCTGTATTAATGCTAACCAAGTCATCGTCAACAACCTAGACAAATCAGCTGGTTTTCCATTTAATAAATGGGGTAAGGCTAGACTTTATTATGATTCAATGAGTTATGAGGATCAAGATGCACTTTTCGCATATACAAAACGTAATGTCATCCCTACTATAACTCAAATGAATCTTAAGTATGCCATTAGTGCAAAGAATAGAGCTCGCACCGTAGCTGGTGTCTCTATCTGTAGTACTATGACCAATAGACAGTTTCATCAAAAATTATTGAAATCAATAGCCGCCACTAGAGGAGCTACTGTAGTAATTGGAACAAGCAAATTCTATGGTGGTTGGCACAACATGTTAAAAACTGTTTATAGTGATGTAGAAAACCCTCACCTTATGGGTTGGGATTATCCTAAATGTGATAGAGCCATGCCTAACATGCTTAGAATTATGGCCTCACTTGTTCTTGCTCGCAAACATACAACGTGTTGTAGCTTGTCACACCGTTTCTATAGATTAGCTAATGAGTGTGCTCAAGTATTGAGTGAAATGGTCATGTGTGGCGGTTCACTATATGTTAAACCAGGTGGAACCTCATCAGGAGATGCCACAACTGCTTATGCTAATAGTGTTTTTAACATTTGTCAAGCTGTCACGGCCAATGTTAATGCACTTTTATCTACTGATGGTAACAAAATTGCCGATAAGTATGTCCGCAATTTA</t>
   </si>
   <si>
@@ -231,15 +228,6 @@
     <t>GGCTATTGATTTCAATAATTTTTGATGAAACTGTCTATTGGTCATAGTACTACAGATA</t>
   </si>
   <si>
-    <t>AACTACAGCCATAACCTTTCCACATACCGCAGACGGTACAGACTGTGTTTTTAAGTGT</t>
-  </si>
-  <si>
-    <t>GGGTTCGCGGAGTTGATCACAACTACAGCCATAACCTTTCCACATACCGCAGACGGTA</t>
-  </si>
-  <si>
-    <t>GCAAAACCAGCTACTTTATCATTGTAGATGTCAAAAGCCCTGTATACGACATCAGTAC</t>
-  </si>
-  <si>
     <t>SARS2_3kb_ASO_1-1</t>
   </si>
   <si>
@@ -540,15 +528,6 @@
     <t>TAAATTGCGGACATACTTATCGGCAATTTTGTTACCATCAGTAGATAAAAGTGC</t>
   </si>
   <si>
-    <t>SARS2_3kb_ASO_FSE-1</t>
-  </si>
-  <si>
-    <t>SARS2_3kb_ASO_FSE-2</t>
-  </si>
-  <si>
-    <t>SARS2_3kb_ASO_FSE-3</t>
-  </si>
-  <si>
     <t>IBV_FT7</t>
   </si>
   <si>
@@ -736,13 +715,16 @@
   </si>
   <si>
     <t>Group</t>
+  </si>
+  <si>
+    <t>SARS2_2924nt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -757,6 +739,17 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
     </font>
   </fonts>
   <fills count="2">
@@ -779,9 +772,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,9 +795,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -840,7 +835,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -946,7 +941,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1088,7 +1083,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1098,8 +1093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69940BED-8353-564B-90FA-E73D0D0C5044}">
   <dimension ref="A1:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1117,210 +1112,210 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
-      </c>
-      <c r="B3" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
         <v>23</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
         <v>25</v>
-      </c>
-      <c r="B8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" t="s">
         <v>33</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
-      </c>
-      <c r="B13" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" t="s">
         <v>37</v>
-      </c>
-      <c r="B14" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
         <v>41</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18" t="s">
         <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" t="s">
         <v>47</v>
-      </c>
-      <c r="B19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B21" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1328,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1351,15 +1346,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1367,10 +1362,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="B3" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -1378,10 +1373,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1389,10 +1384,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B5" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1400,10 +1395,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B6" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -1411,10 +1406,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -1422,10 +1417,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1433,10 +1428,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
       <c r="B9" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1444,10 +1439,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="B10" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -1455,10 +1450,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
       <c r="B11" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -1466,10 +1461,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="B12" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="C12">
         <v>2</v>
@@ -1477,10 +1472,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="B13" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -1488,10 +1483,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -1499,10 +1494,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="C15">
         <v>1</v>
@@ -1510,10 +1505,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="B16" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="C16">
         <v>2</v>
@@ -1521,10 +1516,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="B17" t="s">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="C17">
         <v>1</v>
@@ -1532,10 +1527,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="B18" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="C18">
         <v>2</v>
@@ -1543,10 +1538,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="B19" t="s">
-        <v>204</v>
+        <v>197</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -1554,10 +1549,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="B20" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -1565,10 +1560,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>207</v>
+        <v>200</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>201</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -1576,10 +1571,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="B22" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="C22">
         <v>2</v>
@@ -1587,10 +1582,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
       <c r="B23" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -1598,10 +1593,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="B24" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -1609,10 +1604,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="B25" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="C25">
         <v>1</v>
@@ -1620,10 +1615,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="B26" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="C26">
         <v>2</v>
@@ -1631,10 +1626,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B27" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1642,10 +1637,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C28">
         <v>2</v>
@@ -1653,10 +1648,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>223</v>
+        <v>216</v>
       </c>
       <c r="B29" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -1664,10 +1659,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B30" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1675,10 +1670,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B31" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -1686,10 +1681,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B32" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1701,37 +1696,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92704694-D69F-A540-A91E-639A3FDB18C6}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="255.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B2" s="3">
         <f>LEN(C2)</f>
         <v>2924</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1741,10 +1738,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED6D2C50-7FDD-5044-A66D-CB54A830EB47}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:N1048576"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1758,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1766,674 +1763,638 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B2">
         <f>LEN(C2)</f>
         <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B57" si="0">LEN(C3)</f>
+        <f t="shared" ref="B3:B54" si="0">LEN(C3)</f>
         <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C13" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C21" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C27" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C29" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C30" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C31" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C33" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C34" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C35" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
       <c r="C45" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="C46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="C48" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C50" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C51" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C52" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C53" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="C54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>166</v>
-      </c>
-      <c r="B55">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C55" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" t="s">
-        <v>167</v>
-      </c>
-      <c r="B56">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C56" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>168</v>
-      </c>
-      <c r="B57">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C57" t="s">
-        <v>65</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>